<commit_message>
Casted double to big decimal
</commit_message>
<xml_diff>
--- a/poc-percentage.xlsx
+++ b/poc-percentage.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\jamith\poc-percentage\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -91,11 +91,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -376,19 +379,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.140625" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -396,23 +399,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2.5000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="1">
-        <v>0.124</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1.24E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -420,29 +423,30 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="1">
-        <v>0.34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5" s="6">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="1">
-        <v>0.69</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B6" s="6">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="1">
-        <v>0.01</v>
-      </c>
+      <c r="B7" s="6">
+        <v>2</v>
+      </c>
+      <c r="I7" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>